<commit_message>
Inicie el repositorioremoto en la nube
</commit_message>
<xml_diff>
--- a/Cronograma del mes.xlsx
+++ b/Cronograma del mes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\OneDrive\Escritorio\Informatica Teoria\Calendario de Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{93DE0258-F68E-49EF-99E8-11CF26667B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83E635D-6B5A-4143-9AD6-BDE36578F5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="47">
   <si>
     <t>Hora</t>
   </si>
@@ -418,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1439,7 +1439,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1551,9 @@
       <c r="F5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="H5" s="25" t="s">
         <v>14</v>
       </c>
@@ -1578,7 +1580,9 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="H6" s="25" t="s">
         <v>14</v>
       </c>
@@ -3509,1074 +3513,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
-    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
-                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
-                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
-                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
-                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
-                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
-                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
-                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
-                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
-                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
-                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
-                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
-                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
-                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
-                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
-                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
-                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
-                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
-                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
-                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
-                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
-                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
-                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
-                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
-                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
-                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
-                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
-                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
-                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
-                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
-                <xsd:element ref="ns2:Manager" minOccurs="0"/>
-                <xsd:element ref="ns2:Markets" minOccurs="0"/>
-                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
-                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
-                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
-                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
-                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
-                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
-                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
-                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
-                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
-                <xsd:element ref="ns2:Provider" minOccurs="0"/>
-                <xsd:element ref="ns2:Providers" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
-                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
-                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
-                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
-                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
-                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
-                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
-                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
-                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
-                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
-                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
-                <xsd:element ref="ns3:Description0" minOccurs="0"/>
-                <xsd:element ref="ns3:Component" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Internal MS"/>
-          <xsd:enumeration value="Community"/>
-          <xsd:enumeration value="MVP"/>
-          <xsd:enumeration value="Publisher"/>
-          <xsd:enumeration value="Partner"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="InProgress"/>
-          <xsd:enumeration value="Rejected"/>
-          <xsd:enumeration value="Questionable"/>
-          <xsd:enumeration value="ApprovedAutomatic"/>
-          <xsd:enumeration value="ApprovedManual"/>
-          <xsd:enumeration value="On Hold"/>
-          <xsd:enumeration value="Needs Review"/>
-          <xsd:enumeration value="A Violation"/>
-          <xsd:enumeration value="Unpublished Violation"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Best Bets"/>
-          <xsd:enumeration value="Expire"/>
-          <xsd:enumeration value="Hide"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Template"/>
-          <xsd:enumeration value="Training"/>
-          <xsd:enumeration value="URL"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="14"/>
-          <xsd:enumeration value="15"/>
-          <xsd:enumeration value="16"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Hide on web"/>
-          <xsd:enumeration value="On Web no search"/>
-          <xsd:enumeration value="Show everywhere"/>
-          <xsd:enumeration value="Special use only"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Localize"/>
-          <xsd:enumeration value="Never Localize"/>
-          <xsd:enumeration value="Priority Localize"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Downloads xmlns="2958f784-0ef9-4616-b22d-512a8cad1f0d">0</Downloads>
@@ -4716,7 +3652,1094 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
+    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
+                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
+                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
+                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
+                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
+                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
+                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
+                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
+                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
+                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
+                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
+                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
+                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
+                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
+                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
+                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
+                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
+                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
+                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
+                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
+                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
+                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
+                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
+                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
+                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
+                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
+                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
+                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
+                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
+                <xsd:element ref="ns2:Manager" minOccurs="0"/>
+                <xsd:element ref="ns2:Markets" minOccurs="0"/>
+                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
+                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
+                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
+                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
+                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
+                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
+                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
+                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
+                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
+                <xsd:element ref="ns2:Provider" minOccurs="0"/>
+                <xsd:element ref="ns2:Providers" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
+                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
+                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
+                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
+                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
+                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
+                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
+                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
+                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
+                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
+                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
+                <xsd:element ref="ns3:Description0" minOccurs="0"/>
+                <xsd:element ref="ns3:Component" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Internal MS"/>
+          <xsd:enumeration value="Community"/>
+          <xsd:enumeration value="MVP"/>
+          <xsd:enumeration value="Publisher"/>
+          <xsd:enumeration value="Partner"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="InProgress"/>
+          <xsd:enumeration value="Rejected"/>
+          <xsd:enumeration value="Questionable"/>
+          <xsd:enumeration value="ApprovedAutomatic"/>
+          <xsd:enumeration value="ApprovedManual"/>
+          <xsd:enumeration value="On Hold"/>
+          <xsd:enumeration value="Needs Review"/>
+          <xsd:enumeration value="A Violation"/>
+          <xsd:enumeration value="Unpublished Violation"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Best Bets"/>
+          <xsd:enumeration value="Expire"/>
+          <xsd:enumeration value="Hide"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Template"/>
+          <xsd:enumeration value="Training"/>
+          <xsd:enumeration value="URL"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="14"/>
+          <xsd:enumeration value="15"/>
+          <xsd:enumeration value="16"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Hide on web"/>
+          <xsd:enumeration value="On Web no search"/>
+          <xsd:enumeration value="Show everywhere"/>
+          <xsd:enumeration value="Special use only"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Localize"/>
+          <xsd:enumeration value="Never Localize"/>
+          <xsd:enumeration value="Priority Localize"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E314C6-CC6F-4B8C-BA77-46BFB16C292A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4733,23 +4756,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cambios realizados hasta el 15 de FEB
</commit_message>
<xml_diff>
--- a/Cronograma del mes.xlsx
+++ b/Cronograma del mes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\OneDrive\Escritorio\Informatica Teoria\Calendario de Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83E635D-6B5A-4143-9AD6-BDE36578F5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDD543D-FC36-4535-B617-DE5BA4C4AF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="49">
   <si>
     <t>Hora</t>
   </si>
@@ -170,13 +170,19 @@
   </si>
   <si>
     <t xml:space="preserve">SEMANA 4: DEL LUNES 6 DE MARZO AL DOMINGO 12 DE MARZO </t>
+  </si>
+  <si>
+    <t>ORGANIZAR PARA LA CITA</t>
+  </si>
+  <si>
+    <t>CITA QUE NO RECORDABA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +207,13 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -343,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -420,6 +433,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1438,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA15572-563F-4C9E-BFF5-DC1E6F276711}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,13 +1507,11 @@
       <c r="A3" s="6">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>2</v>
+      <c r="B3" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="24"/>
-      <c r="D3" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="D3" s="16"/>
       <c r="E3" s="23" t="s">
         <v>13</v>
       </c>
@@ -1511,14 +1525,14 @@
       <c r="A4" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>2</v>
+      <c r="B4" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>2</v>
+      <c r="D4" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>5</v>
@@ -1536,14 +1550,14 @@
       <c r="A5" s="6">
         <v>0.375</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>2</v>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>2</v>
+      <c r="D5" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>5</v>
@@ -1551,9 +1565,7 @@
       <c r="F5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>22</v>
-      </c>
+      <c r="G5" s="26"/>
       <c r="H5" s="25" t="s">
         <v>14</v>
       </c>
@@ -1565,8 +1577,8 @@
       <c r="A6" s="6">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>3</v>
+      <c r="B6" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>5</v>
@@ -1580,9 +1592,7 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="26" t="s">
-        <v>22</v>
-      </c>
+      <c r="G6" s="26"/>
       <c r="H6" s="25" t="s">
         <v>14</v>
       </c>
@@ -1594,8 +1604,8 @@
       <c r="A7" s="6">
         <v>0.45833333333333398</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>3</v>
+      <c r="B7" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>7</v>
@@ -1621,8 +1631,8 @@
       <c r="A8" s="6">
         <v>0.5</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>3</v>
+      <c r="B8" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>7</v>
@@ -1651,8 +1661,8 @@
       <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>12</v>
+      <c r="C9" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>9</v>
@@ -1678,11 +1688,11 @@
       <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>12</v>
+      <c r="C10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>12</v>
@@ -1705,11 +1715,11 @@
       <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>12</v>
+      <c r="C11" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>12</v>
@@ -1732,11 +1742,11 @@
       <c r="B12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>12</v>
+      <c r="C12" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>6</v>
@@ -1756,11 +1766,11 @@
       <c r="A13" s="6">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>3</v>
+      <c r="B13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>3</v>
@@ -1781,8 +1791,8 @@
       <c r="A14" s="6">
         <v>0.75</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>12</v>
+      <c r="B14" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>12</v>
@@ -1806,14 +1816,14 @@
       <c r="A15" s="6">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>3</v>
+      <c r="B15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>12</v>
@@ -1834,11 +1844,11 @@
       <c r="B16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>3</v>
+      <c r="C16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Cambios realizados hasta el 19 FEB
</commit_message>
<xml_diff>
--- a/Cronograma del mes.xlsx
+++ b/Cronograma del mes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\OneDrive\Escritorio\Informatica Teoria\Calendario de Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDD543D-FC36-4535-B617-DE5BA4C4AF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538C8282-D83D-4406-8C9A-98830C08A472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="50">
   <si>
     <t>Hora</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>CITA QUE NO RECORDABA</t>
+  </si>
+  <si>
+    <t>AYUDAR EN LA CASA</t>
   </si>
 </sst>
 </file>
@@ -1454,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA15572-563F-4C9E-BFF5-DC1E6F276711}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,11 +1518,9 @@
       <c r="E3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -1537,11 +1538,11 @@
       <c r="E4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
+      <c r="F4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="J4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1562,10 +1563,12 @@
       <c r="E5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="26"/>
+      <c r="F5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="H5" s="25" t="s">
         <v>14</v>
       </c>
@@ -1592,7 +1595,9 @@
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="H6" s="25" t="s">
         <v>14</v>
       </c>
@@ -1619,7 +1624,9 @@
       <c r="F7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="H7" s="25" t="s">
         <v>14</v>
       </c>
@@ -1646,7 +1653,9 @@
       <c r="F8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H8" s="25" t="s">
         <v>14</v>
       </c>
@@ -1667,13 +1676,15 @@
       <c r="D9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>12</v>
+      <c r="E9" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H9" s="25" t="s">
         <v>14</v>
       </c>
@@ -1700,7 +1711,9 @@
       <c r="F10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="25" t="s">
         <v>14</v>
       </c>
@@ -1727,7 +1740,9 @@
       <c r="F11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="H11" s="25" t="s">
         <v>14</v>
       </c>
@@ -1754,7 +1769,9 @@
       <c r="F12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H12" s="25" t="s">
         <v>14</v>
       </c>
@@ -1781,8 +1798,12 @@
       <c r="F13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="4"/>
+      <c r="G13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="J13" s="16" t="s">
         <v>12</v>
       </c>
@@ -1803,11 +1824,15 @@
       <c r="E14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="4"/>
+      <c r="F14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="J14" s="25" t="s">
         <v>14</v>
       </c>
@@ -1828,11 +1853,15 @@
       <c r="E15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="J15" s="26" t="s">
         <v>22</v>
       </c>
@@ -1850,14 +1879,18 @@
       <c r="D16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>12</v>
+      <c r="E16" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
@@ -1878,8 +1911,12 @@
       <c r="F17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="4"/>
+      <c r="G17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
@@ -3523,6 +3560,1074 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
+    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
+                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
+                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
+                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
+                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
+                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
+                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
+                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
+                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
+                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
+                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
+                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
+                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
+                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
+                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
+                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
+                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
+                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
+                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
+                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
+                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
+                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
+                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
+                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
+                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
+                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
+                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
+                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
+                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
+                <xsd:element ref="ns2:Manager" minOccurs="0"/>
+                <xsd:element ref="ns2:Markets" minOccurs="0"/>
+                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
+                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
+                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
+                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
+                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
+                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
+                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
+                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
+                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
+                <xsd:element ref="ns2:Provider" minOccurs="0"/>
+                <xsd:element ref="ns2:Providers" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
+                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
+                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
+                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
+                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
+                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
+                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
+                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
+                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
+                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
+                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
+                <xsd:element ref="ns3:Description0" minOccurs="0"/>
+                <xsd:element ref="ns3:Component" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Internal MS"/>
+          <xsd:enumeration value="Community"/>
+          <xsd:enumeration value="MVP"/>
+          <xsd:enumeration value="Publisher"/>
+          <xsd:enumeration value="Partner"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="InProgress"/>
+          <xsd:enumeration value="Rejected"/>
+          <xsd:enumeration value="Questionable"/>
+          <xsd:enumeration value="ApprovedAutomatic"/>
+          <xsd:enumeration value="ApprovedManual"/>
+          <xsd:enumeration value="On Hold"/>
+          <xsd:enumeration value="Needs Review"/>
+          <xsd:enumeration value="A Violation"/>
+          <xsd:enumeration value="Unpublished Violation"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Best Bets"/>
+          <xsd:enumeration value="Expire"/>
+          <xsd:enumeration value="Hide"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Template"/>
+          <xsd:enumeration value="Training"/>
+          <xsd:enumeration value="URL"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="14"/>
+          <xsd:enumeration value="15"/>
+          <xsd:enumeration value="16"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Hide on web"/>
+          <xsd:enumeration value="On Web no search"/>
+          <xsd:enumeration value="Show everywhere"/>
+          <xsd:enumeration value="Special use only"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Localize"/>
+          <xsd:enumeration value="Never Localize"/>
+          <xsd:enumeration value="Priority Localize"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Downloads xmlns="2958f784-0ef9-4616-b22d-512a8cad1f0d">0</Downloads>
@@ -3662,1094 +4767,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
-    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
-                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
-                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
-                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
-                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
-                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
-                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
-                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
-                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
-                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
-                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
-                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
-                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
-                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
-                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
-                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
-                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
-                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
-                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
-                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
-                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
-                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
-                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
-                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
-                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
-                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
-                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
-                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
-                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
-                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
-                <xsd:element ref="ns2:Manager" minOccurs="0"/>
-                <xsd:element ref="ns2:Markets" minOccurs="0"/>
-                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
-                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
-                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
-                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
-                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
-                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
-                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
-                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
-                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
-                <xsd:element ref="ns2:Provider" minOccurs="0"/>
-                <xsd:element ref="ns2:Providers" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
-                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
-                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
-                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
-                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
-                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
-                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
-                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
-                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
-                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
-                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
-                <xsd:element ref="ns3:Description0" minOccurs="0"/>
-                <xsd:element ref="ns3:Component" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Internal MS"/>
-          <xsd:enumeration value="Community"/>
-          <xsd:enumeration value="MVP"/>
-          <xsd:enumeration value="Publisher"/>
-          <xsd:enumeration value="Partner"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="InProgress"/>
-          <xsd:enumeration value="Rejected"/>
-          <xsd:enumeration value="Questionable"/>
-          <xsd:enumeration value="ApprovedAutomatic"/>
-          <xsd:enumeration value="ApprovedManual"/>
-          <xsd:enumeration value="On Hold"/>
-          <xsd:enumeration value="Needs Review"/>
-          <xsd:enumeration value="A Violation"/>
-          <xsd:enumeration value="Unpublished Violation"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Best Bets"/>
-          <xsd:enumeration value="Expire"/>
-          <xsd:enumeration value="Hide"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Template"/>
-          <xsd:enumeration value="Training"/>
-          <xsd:enumeration value="URL"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="14"/>
-          <xsd:enumeration value="15"/>
-          <xsd:enumeration value="16"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Hide on web"/>
-          <xsd:enumeration value="On Web no search"/>
-          <xsd:enumeration value="Show everywhere"/>
-          <xsd:enumeration value="Special use only"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Localize"/>
-          <xsd:enumeration value="Never Localize"/>
-          <xsd:enumeration value="Priority Localize"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E314C6-CC6F-4B8C-BA77-46BFB16C292A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4766,4 +4784,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cambios realizados hasta el 21 FEB
</commit_message>
<xml_diff>
--- a/Cronograma del mes.xlsx
+++ b/Cronograma del mes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\OneDrive\Escritorio\Informatica Teoria\Calendario de Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538C8282-D83D-4406-8C9A-98830C08A472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13513B95-2C16-4E40-9055-42B49DF6B227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="52">
   <si>
     <t>Hora</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>AYUDAR EN LA CASA</t>
+  </si>
+  <si>
+    <t>CITA PUNTOS CORDAL</t>
+  </si>
+  <si>
+    <t>CITA ORTODONCIA</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA15572-563F-4C9E-BFF5-DC1E6F276711}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -2009,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2D5547-40E9-4E82-8994-0832A696D7AB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,9 +2068,7 @@
       <c r="A3" s="6">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="D3" s="12" t="s">
         <v>2</v>
@@ -2080,9 +2084,7 @@
       <c r="A4" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="B4" s="24"/>
       <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
@@ -2105,8 +2107,8 @@
       <c r="A5" s="6">
         <v>0.375</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>2</v>
+      <c r="B5" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>5</v>
@@ -2132,8 +2134,8 @@
       <c r="A6" s="6">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>3</v>
+      <c r="B6" s="23" t="s">
+        <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>5</v>
@@ -2159,8 +2161,8 @@
       <c r="A7" s="6">
         <v>0.45833333333333398</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>3</v>
+      <c r="B7" s="23" t="s">
+        <v>51</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>7</v>
@@ -2186,8 +2188,8 @@
       <c r="A8" s="6">
         <v>0.5</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>3</v>
+      <c r="B8" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>7</v>
@@ -2349,8 +2351,8 @@
       <c r="B14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>12</v>
+      <c r="C14" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>3</v>
@@ -2374,8 +2376,8 @@
       <c r="B15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>12</v>
+      <c r="C15" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>3</v>
@@ -2399,8 +2401,8 @@
       <c r="B16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>12</v>
+      <c r="C16" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>3</v>
@@ -2443,8 +2445,8 @@
       <c r="B18" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>11</v>
+      <c r="C18" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>11</v>
@@ -3560,1074 +3562,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
-    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
-                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
-                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
-                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
-                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
-                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
-                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
-                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
-                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
-                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
-                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
-                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
-                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
-                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
-                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
-                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
-                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
-                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
-                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
-                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
-                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
-                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
-                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
-                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
-                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
-                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
-                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
-                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
-                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
-                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
-                <xsd:element ref="ns2:Manager" minOccurs="0"/>
-                <xsd:element ref="ns2:Markets" minOccurs="0"/>
-                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
-                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
-                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
-                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
-                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
-                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
-                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
-                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
-                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
-                <xsd:element ref="ns2:Provider" minOccurs="0"/>
-                <xsd:element ref="ns2:Providers" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
-                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
-                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
-                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
-                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
-                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
-                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
-                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
-                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
-                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
-                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
-                <xsd:element ref="ns3:Description0" minOccurs="0"/>
-                <xsd:element ref="ns3:Component" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Internal MS"/>
-          <xsd:enumeration value="Community"/>
-          <xsd:enumeration value="MVP"/>
-          <xsd:enumeration value="Publisher"/>
-          <xsd:enumeration value="Partner"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="InProgress"/>
-          <xsd:enumeration value="Rejected"/>
-          <xsd:enumeration value="Questionable"/>
-          <xsd:enumeration value="ApprovedAutomatic"/>
-          <xsd:enumeration value="ApprovedManual"/>
-          <xsd:enumeration value="On Hold"/>
-          <xsd:enumeration value="Needs Review"/>
-          <xsd:enumeration value="A Violation"/>
-          <xsd:enumeration value="Unpublished Violation"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Best Bets"/>
-          <xsd:enumeration value="Expire"/>
-          <xsd:enumeration value="Hide"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Template"/>
-          <xsd:enumeration value="Training"/>
-          <xsd:enumeration value="URL"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="14"/>
-          <xsd:enumeration value="15"/>
-          <xsd:enumeration value="16"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Hide on web"/>
-          <xsd:enumeration value="On Web no search"/>
-          <xsd:enumeration value="Show everywhere"/>
-          <xsd:enumeration value="Special use only"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Localize"/>
-          <xsd:enumeration value="Never Localize"/>
-          <xsd:enumeration value="Priority Localize"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Downloads xmlns="2958f784-0ef9-4616-b22d-512a8cad1f0d">0</Downloads>
@@ -4767,7 +3701,1094 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
+    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
+                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
+                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
+                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
+                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
+                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
+                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
+                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
+                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
+                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
+                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
+                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
+                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
+                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
+                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
+                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
+                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
+                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
+                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
+                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
+                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
+                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
+                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
+                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
+                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
+                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
+                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
+                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
+                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
+                <xsd:element ref="ns2:Manager" minOccurs="0"/>
+                <xsd:element ref="ns2:Markets" minOccurs="0"/>
+                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
+                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
+                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
+                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
+                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
+                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
+                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
+                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
+                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
+                <xsd:element ref="ns2:Provider" minOccurs="0"/>
+                <xsd:element ref="ns2:Providers" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
+                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
+                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
+                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
+                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
+                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
+                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
+                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
+                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
+                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
+                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
+                <xsd:element ref="ns3:Description0" minOccurs="0"/>
+                <xsd:element ref="ns3:Component" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Internal MS"/>
+          <xsd:enumeration value="Community"/>
+          <xsd:enumeration value="MVP"/>
+          <xsd:enumeration value="Publisher"/>
+          <xsd:enumeration value="Partner"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="InProgress"/>
+          <xsd:enumeration value="Rejected"/>
+          <xsd:enumeration value="Questionable"/>
+          <xsd:enumeration value="ApprovedAutomatic"/>
+          <xsd:enumeration value="ApprovedManual"/>
+          <xsd:enumeration value="On Hold"/>
+          <xsd:enumeration value="Needs Review"/>
+          <xsd:enumeration value="A Violation"/>
+          <xsd:enumeration value="Unpublished Violation"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Best Bets"/>
+          <xsd:enumeration value="Expire"/>
+          <xsd:enumeration value="Hide"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Template"/>
+          <xsd:enumeration value="Training"/>
+          <xsd:enumeration value="URL"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="14"/>
+          <xsd:enumeration value="15"/>
+          <xsd:enumeration value="16"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Hide on web"/>
+          <xsd:enumeration value="On Web no search"/>
+          <xsd:enumeration value="Show everywhere"/>
+          <xsd:enumeration value="Special use only"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Localize"/>
+          <xsd:enumeration value="Never Localize"/>
+          <xsd:enumeration value="Priority Localize"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E314C6-CC6F-4B8C-BA77-46BFB16C292A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4784,23 +4805,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se le quito una hora a las actividades de entrenar y estudiar, como lo pidio el profesor en la clase del 21 de febrero
</commit_message>
<xml_diff>
--- a/Cronograma del mes.xlsx
+++ b/Cronograma del mes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\OneDrive\Escritorio\Informatica Teoria\Calendario de Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13513B95-2C16-4E40-9055-42B49DF6B227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F19CA4C-EA85-493F-A6B0-95498AC1F864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="52">
   <si>
     <t>Hora</t>
   </si>
@@ -2015,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2D5547-40E9-4E82-8994-0832A696D7AB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,9 +2070,7 @@
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
-      <c r="D3" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="12" t="s">
         <v>2</v>
@@ -2119,8 +2117,8 @@
       <c r="E5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>2</v>
+      <c r="F5" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="25" t="s">
@@ -2335,8 +2333,8 @@
       <c r="E13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>3</v>
+      <c r="F13" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="4"/>
@@ -2404,8 +2402,8 @@
       <c r="C16" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>3</v>
+      <c r="D16" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>12</v>
@@ -2530,7 +2528,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,16 +2580,16 @@
       <c r="A3" s="6">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>2</v>
+      <c r="B3" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="24"/>
-      <c r="D3" s="12" t="s">
-        <v>2</v>
+      <c r="D3" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="E3" s="16"/>
-      <c r="F3" s="12" t="s">
-        <v>2</v>
+      <c r="F3" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="4"/>
@@ -2706,8 +2704,8 @@
       <c r="A8" s="6">
         <v>0.5</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>3</v>
+      <c r="B8" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>7</v>
@@ -2790,8 +2788,8 @@
       <c r="B11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>3</v>
+      <c r="C11" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>12</v>
@@ -2799,8 +2797,8 @@
       <c r="E11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>3</v>
+      <c r="F11" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="25" t="s">
@@ -2847,8 +2845,8 @@
       <c r="C13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>3</v>
+      <c r="D13" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>6</v>
@@ -3047,8 +3045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3E4226-4CC4-4FC9-BB07-3237BB0548E8}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,12 +3098,12 @@
       <c r="A3" s="6">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>2</v>
+      <c r="B3" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="24"/>
-      <c r="D3" s="12" t="s">
-        <v>2</v>
+      <c r="D3" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="12" t="s">
@@ -3224,8 +3222,8 @@
       <c r="A8" s="6">
         <v>0.5</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>3</v>
+      <c r="B8" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>7</v>
@@ -3308,8 +3306,8 @@
       <c r="B11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>3</v>
+      <c r="C11" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>12</v>
@@ -3317,8 +3315,8 @@
       <c r="E11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>3</v>
+      <c r="F11" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="25" t="s">
@@ -3365,8 +3363,8 @@
       <c r="C13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>3</v>
+      <c r="D13" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>6</v>
@@ -3562,6 +3560,1074 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
+    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
+                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
+                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
+                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
+                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
+                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
+                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
+                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
+                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
+                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
+                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
+                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
+                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
+                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
+                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
+                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
+                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
+                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
+                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
+                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
+                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
+                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
+                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
+                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
+                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
+                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
+                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
+                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
+                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
+                <xsd:element ref="ns2:Manager" minOccurs="0"/>
+                <xsd:element ref="ns2:Markets" minOccurs="0"/>
+                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
+                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
+                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
+                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
+                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
+                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
+                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
+                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
+                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
+                <xsd:element ref="ns2:Provider" minOccurs="0"/>
+                <xsd:element ref="ns2:Providers" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
+                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
+                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
+                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
+                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
+                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
+                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
+                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
+                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
+                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
+                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
+                <xsd:element ref="ns3:Description0" minOccurs="0"/>
+                <xsd:element ref="ns3:Component" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Internal MS"/>
+          <xsd:enumeration value="Community"/>
+          <xsd:enumeration value="MVP"/>
+          <xsd:enumeration value="Publisher"/>
+          <xsd:enumeration value="Partner"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="InProgress"/>
+          <xsd:enumeration value="Rejected"/>
+          <xsd:enumeration value="Questionable"/>
+          <xsd:enumeration value="ApprovedAutomatic"/>
+          <xsd:enumeration value="ApprovedManual"/>
+          <xsd:enumeration value="On Hold"/>
+          <xsd:enumeration value="Needs Review"/>
+          <xsd:enumeration value="A Violation"/>
+          <xsd:enumeration value="Unpublished Violation"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Best Bets"/>
+          <xsd:enumeration value="Expire"/>
+          <xsd:enumeration value="Hide"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Template"/>
+          <xsd:enumeration value="Training"/>
+          <xsd:enumeration value="URL"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="14"/>
+          <xsd:enumeration value="15"/>
+          <xsd:enumeration value="16"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Hide on web"/>
+          <xsd:enumeration value="On Web no search"/>
+          <xsd:enumeration value="Show everywhere"/>
+          <xsd:enumeration value="Special use only"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Localize"/>
+          <xsd:enumeration value="Never Localize"/>
+          <xsd:enumeration value="Priority Localize"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Downloads xmlns="2958f784-0ef9-4616-b22d-512a8cad1f0d">0</Downloads>
@@ -3701,1094 +4767,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
-    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
-                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
-                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
-                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
-                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
-                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
-                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
-                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
-                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
-                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
-                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
-                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
-                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
-                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
-                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
-                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
-                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
-                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
-                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
-                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
-                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
-                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
-                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
-                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
-                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
-                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
-                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
-                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
-                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
-                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
-                <xsd:element ref="ns2:Manager" minOccurs="0"/>
-                <xsd:element ref="ns2:Markets" minOccurs="0"/>
-                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
-                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
-                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
-                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
-                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
-                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
-                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
-                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
-                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
-                <xsd:element ref="ns2:Provider" minOccurs="0"/>
-                <xsd:element ref="ns2:Providers" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
-                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
-                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
-                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
-                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
-                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
-                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
-                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
-                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
-                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
-                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
-                <xsd:element ref="ns3:Description0" minOccurs="0"/>
-                <xsd:element ref="ns3:Component" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Internal MS"/>
-          <xsd:enumeration value="Community"/>
-          <xsd:enumeration value="MVP"/>
-          <xsd:enumeration value="Publisher"/>
-          <xsd:enumeration value="Partner"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="InProgress"/>
-          <xsd:enumeration value="Rejected"/>
-          <xsd:enumeration value="Questionable"/>
-          <xsd:enumeration value="ApprovedAutomatic"/>
-          <xsd:enumeration value="ApprovedManual"/>
-          <xsd:enumeration value="On Hold"/>
-          <xsd:enumeration value="Needs Review"/>
-          <xsd:enumeration value="A Violation"/>
-          <xsd:enumeration value="Unpublished Violation"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Best Bets"/>
-          <xsd:enumeration value="Expire"/>
-          <xsd:enumeration value="Hide"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Template"/>
-          <xsd:enumeration value="Training"/>
-          <xsd:enumeration value="URL"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="14"/>
-          <xsd:enumeration value="15"/>
-          <xsd:enumeration value="16"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Hide on web"/>
-          <xsd:enumeration value="On Web no search"/>
-          <xsd:enumeration value="Show everywhere"/>
-          <xsd:enumeration value="Special use only"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Localize"/>
-          <xsd:enumeration value="Never Localize"/>
-          <xsd:enumeration value="Priority Localize"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E314C6-CC6F-4B8C-BA77-46BFB16C292A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4805,4 +4784,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cambios realizados hasta el 26 FEB
</commit_message>
<xml_diff>
--- a/Cronograma del mes.xlsx
+++ b/Cronograma del mes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\OneDrive\Escritorio\Informatica Teoria\Calendario de Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F19CA4C-EA85-493F-A6B0-95498AC1F864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3495F7F3-ADF5-497E-88FA-2220B9EE588E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="54">
   <si>
     <t>Hora</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>CITA ORTODONCIA</t>
+  </si>
+  <si>
+    <t>ORGANIZAR PARA IR AL LAB</t>
+  </si>
+  <si>
+    <t>AYUDAR EN CASA</t>
   </si>
 </sst>
 </file>
@@ -2015,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2D5547-40E9-4E82-8994-0832A696D7AB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,9 +2092,7 @@
       <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="D4" s="16"/>
       <c r="E4" s="18" t="s">
         <v>5</v>
       </c>
@@ -2111,14 +2115,12 @@
       <c r="C5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="D5" s="16"/>
       <c r="E5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>22</v>
+      <c r="F5" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="25" t="s">
@@ -2201,7 +2203,9 @@
       <c r="F8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="H8" s="25" t="s">
         <v>14</v>
       </c>
@@ -2219,8 +2223,8 @@
       <c r="C9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>9</v>
+      <c r="D9" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>12</v>
@@ -2228,7 +2232,9 @@
       <c r="F9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="H9" s="25" t="s">
         <v>14</v>
       </c>
@@ -2246,8 +2252,8 @@
       <c r="C10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>12</v>
+      <c r="D10" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>12</v>
@@ -2276,8 +2282,8 @@
       <c r="D11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>12</v>
+      <c r="E11" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>3</v>
@@ -2327,16 +2333,18 @@
       <c r="C13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>3</v>
+      <c r="D13" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="5"/>
+      <c r="F13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="J13" s="16" t="s">
         <v>12</v>
@@ -2352,16 +2360,18 @@
       <c r="C14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>3</v>
+      <c r="D14" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="5"/>
+      <c r="F14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="J14" s="25" t="s">
         <v>14</v>
@@ -2377,16 +2387,18 @@
       <c r="C15" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>12</v>
+      <c r="D15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="J15" s="26" t="s">
         <v>22</v>
@@ -2402,16 +2414,18 @@
       <c r="C16" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>12</v>
+      <c r="D16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -2424,8 +2438,8 @@
       <c r="C17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>12</v>
+      <c r="D17" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>12</v>
@@ -2433,7 +2447,9 @@
       <c r="F17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -2446,8 +2462,8 @@
       <c r="C18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>11</v>
+      <c r="D18" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>11</v>
@@ -2472,8 +2488,8 @@
       <c r="C19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>11</v>
+      <c r="D19" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>11</v>
@@ -3045,7 +3061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3E4226-4CC4-4FC9-BB07-3237BB0548E8}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -3560,1074 +3576,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
-    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
-                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
-                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
-                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
-                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
-                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
-                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
-                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
-                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
-                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
-                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
-                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
-                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
-                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
-                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
-                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
-                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
-                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
-                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
-                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
-                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
-                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
-                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
-                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
-                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
-                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
-                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
-                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
-                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
-                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
-                <xsd:element ref="ns2:Manager" minOccurs="0"/>
-                <xsd:element ref="ns2:Markets" minOccurs="0"/>
-                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
-                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
-                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
-                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
-                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
-                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
-                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
-                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
-                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
-                <xsd:element ref="ns2:Provider" minOccurs="0"/>
-                <xsd:element ref="ns2:Providers" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
-                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
-                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
-                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
-                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
-                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
-                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
-                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
-                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
-                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
-                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
-                <xsd:element ref="ns3:Description0" minOccurs="0"/>
-                <xsd:element ref="ns3:Component" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Internal MS"/>
-          <xsd:enumeration value="Community"/>
-          <xsd:enumeration value="MVP"/>
-          <xsd:enumeration value="Publisher"/>
-          <xsd:enumeration value="Partner"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="InProgress"/>
-          <xsd:enumeration value="Rejected"/>
-          <xsd:enumeration value="Questionable"/>
-          <xsd:enumeration value="ApprovedAutomatic"/>
-          <xsd:enumeration value="ApprovedManual"/>
-          <xsd:enumeration value="On Hold"/>
-          <xsd:enumeration value="Needs Review"/>
-          <xsd:enumeration value="A Violation"/>
-          <xsd:enumeration value="Unpublished Violation"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Best Bets"/>
-          <xsd:enumeration value="Expire"/>
-          <xsd:enumeration value="Hide"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Template"/>
-          <xsd:enumeration value="Training"/>
-          <xsd:enumeration value="URL"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="14"/>
-          <xsd:enumeration value="15"/>
-          <xsd:enumeration value="16"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Hide on web"/>
-          <xsd:enumeration value="On Web no search"/>
-          <xsd:enumeration value="Show everywhere"/>
-          <xsd:enumeration value="Special use only"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Localize"/>
-          <xsd:enumeration value="Never Localize"/>
-          <xsd:enumeration value="Priority Localize"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Downloads xmlns="2958f784-0ef9-4616-b22d-512a8cad1f0d">0</Downloads>
@@ -4767,7 +3715,1094 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
+    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
+                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
+                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
+                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
+                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
+                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
+                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
+                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
+                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
+                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
+                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
+                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
+                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
+                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
+                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
+                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
+                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
+                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
+                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
+                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
+                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
+                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
+                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
+                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
+                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
+                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
+                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
+                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
+                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
+                <xsd:element ref="ns2:Manager" minOccurs="0"/>
+                <xsd:element ref="ns2:Markets" minOccurs="0"/>
+                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
+                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
+                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
+                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
+                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
+                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
+                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
+                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
+                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
+                <xsd:element ref="ns2:Provider" minOccurs="0"/>
+                <xsd:element ref="ns2:Providers" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
+                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
+                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
+                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
+                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
+                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
+                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
+                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
+                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
+                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
+                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
+                <xsd:element ref="ns3:Description0" minOccurs="0"/>
+                <xsd:element ref="ns3:Component" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Internal MS"/>
+          <xsd:enumeration value="Community"/>
+          <xsd:enumeration value="MVP"/>
+          <xsd:enumeration value="Publisher"/>
+          <xsd:enumeration value="Partner"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="InProgress"/>
+          <xsd:enumeration value="Rejected"/>
+          <xsd:enumeration value="Questionable"/>
+          <xsd:enumeration value="ApprovedAutomatic"/>
+          <xsd:enumeration value="ApprovedManual"/>
+          <xsd:enumeration value="On Hold"/>
+          <xsd:enumeration value="Needs Review"/>
+          <xsd:enumeration value="A Violation"/>
+          <xsd:enumeration value="Unpublished Violation"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Best Bets"/>
+          <xsd:enumeration value="Expire"/>
+          <xsd:enumeration value="Hide"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Template"/>
+          <xsd:enumeration value="Training"/>
+          <xsd:enumeration value="URL"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="14"/>
+          <xsd:enumeration value="15"/>
+          <xsd:enumeration value="16"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Hide on web"/>
+          <xsd:enumeration value="On Web no search"/>
+          <xsd:enumeration value="Show everywhere"/>
+          <xsd:enumeration value="Special use only"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Localize"/>
+          <xsd:enumeration value="Never Localize"/>
+          <xsd:enumeration value="Priority Localize"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E314C6-CC6F-4B8C-BA77-46BFB16C292A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4784,23 +4819,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cambios realizados hasta el 5 de Marzo
</commit_message>
<xml_diff>
--- a/Cronograma del mes.xlsx
+++ b/Cronograma del mes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josed\OneDrive\Escritorio\Informatica Teoria\Calendario de Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3495F7F3-ADF5-497E-88FA-2220B9EE588E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E04C945-0052-42E6-940B-4079C0358EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="61">
   <si>
     <t>Hora</t>
   </si>
@@ -191,6 +191,27 @@
   </si>
   <si>
     <t>AYUDAR EN CASA</t>
+  </si>
+  <si>
+    <t>JUGAR FUTBOL</t>
+  </si>
+  <si>
+    <t>CLASE GUITARRA</t>
+  </si>
+  <si>
+    <t>CITA DE LIMPIEZA</t>
+  </si>
+  <si>
+    <t>TIEMPO EN FAMILIA</t>
+  </si>
+  <si>
+    <t>CLASE PDS-Parcial</t>
+  </si>
+  <si>
+    <t>CLASE OPTI-Quiz</t>
+  </si>
+  <si>
+    <t>LAB INFO-Sutentacion</t>
   </si>
 </sst>
 </file>
@@ -235,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +353,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -371,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,6 +477,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1470,7 +1500,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,7 +2051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2D5547-40E9-4E82-8994-0832A696D7AB}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -2544,14 +2574,14 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="8" width="22.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2596,17 +2626,13 @@
       <c r="A3" s="6">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>22</v>
-      </c>
+      <c r="B3" s="24"/>
       <c r="C3" s="24"/>
-      <c r="D3" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="26" t="s">
-        <v>22</v>
-      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="24"/>
       <c r="G3" s="5"/>
       <c r="H3" s="4"/>
     </row>
@@ -2614,22 +2640,22 @@
       <c r="A4" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="B4" s="24"/>
       <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>5</v>
+      <c r="E4" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="J4" s="12" t="s">
         <v>2</v>
@@ -2639,8 +2665,8 @@
       <c r="A5" s="6">
         <v>0.375</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>2</v>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>5</v>
@@ -2648,13 +2674,15 @@
       <c r="D5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>5</v>
+      <c r="E5" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H5" s="25" t="s">
         <v>14</v>
       </c>
@@ -2675,13 +2703,15 @@
       <c r="D6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>5</v>
+      <c r="E6" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H6" s="25" t="s">
         <v>14</v>
       </c>
@@ -2708,7 +2738,9 @@
       <c r="F7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H7" s="25" t="s">
         <v>14</v>
       </c>
@@ -2720,8 +2752,8 @@
       <c r="A8" s="6">
         <v>0.5</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>22</v>
+      <c r="B8" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>7</v>
@@ -2735,7 +2767,9 @@
       <c r="F8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H8" s="25" t="s">
         <v>14</v>
       </c>
@@ -2756,13 +2790,15 @@
       <c r="D9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>12</v>
+      <c r="E9" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H9" s="25" t="s">
         <v>14</v>
       </c>
@@ -2777,8 +2813,8 @@
       <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>12</v>
+      <c r="C10" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>12</v>
@@ -2789,7 +2825,9 @@
       <c r="F10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H10" s="25" t="s">
         <v>14</v>
       </c>
@@ -2804,19 +2842,21 @@
       <c r="B11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="5"/>
+      <c r="C11" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H11" s="25" t="s">
         <v>14</v>
       </c>
@@ -2831,19 +2871,21 @@
       <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>12</v>
+      <c r="C12" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="F12" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H12" s="25" t="s">
         <v>14</v>
       </c>
@@ -2858,19 +2900,21 @@
       <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>22</v>
+      <c r="C13" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="5"/>
+      <c r="F13" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="J13" s="16" t="s">
         <v>12</v>
@@ -2892,10 +2936,12 @@
       <c r="E14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="5"/>
+      <c r="F14" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="J14" s="25" t="s">
         <v>14</v>
@@ -2905,11 +2951,11 @@
       <c r="A15" s="6">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>12</v>
+      <c r="B15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>3</v>
@@ -2917,10 +2963,12 @@
       <c r="E15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="5"/>
+      <c r="F15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="J15" s="26" t="s">
         <v>22</v>
@@ -2930,11 +2978,11 @@
       <c r="A16" s="6">
         <v>0.83333333333333304</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>12</v>
+      <c r="B16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>3</v>
@@ -2942,11 +2990,14 @@
       <c r="E16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>12</v>
+      <c r="F16" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="4"/>
+      <c r="J16" s="28" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
@@ -2958,14 +3009,14 @@
       <c r="C17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>12</v>
+      <c r="D17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
@@ -3061,8 +3112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3E4226-4CC4-4FC9-BB07-3237BB0548E8}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3197,7 +3248,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="25" t="s">
@@ -3221,10 +3272,10 @@
         <v>9</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="25" t="s">
@@ -3248,10 +3299,10 @@
         <v>9</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="25" t="s">
@@ -3278,7 +3329,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="25" t="s">
@@ -3356,7 +3407,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>3</v>
@@ -3383,7 +3434,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>3</v>
@@ -3408,7 +3459,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>12</v>
@@ -3576,6 +3627,1074 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
+    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
+                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
+                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
+                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
+                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
+                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
+                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
+                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
+                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
+                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
+                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
+                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
+                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
+                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
+                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
+                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
+                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
+                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
+                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
+                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
+                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
+                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
+                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
+                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
+                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
+                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
+                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
+                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
+                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
+                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
+                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
+                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
+                <xsd:element ref="ns2:Manager" minOccurs="0"/>
+                <xsd:element ref="ns2:Markets" minOccurs="0"/>
+                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
+                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
+                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
+                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
+                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
+                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
+                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
+                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
+                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
+                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
+                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
+                <xsd:element ref="ns2:Provider" minOccurs="0"/>
+                <xsd:element ref="ns2:Providers" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
+                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
+                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
+                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
+                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
+                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
+                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
+                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
+                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
+                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
+                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
+                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
+                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
+                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
+                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
+                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
+                <xsd:element ref="ns3:Description0" minOccurs="0"/>
+                <xsd:element ref="ns3:Component" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Internal MS"/>
+          <xsd:enumeration value="Community"/>
+          <xsd:enumeration value="MVP"/>
+          <xsd:enumeration value="Publisher"/>
+          <xsd:enumeration value="Partner"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="InProgress"/>
+          <xsd:enumeration value="Rejected"/>
+          <xsd:enumeration value="Questionable"/>
+          <xsd:enumeration value="ApprovedAutomatic"/>
+          <xsd:enumeration value="ApprovedManual"/>
+          <xsd:enumeration value="On Hold"/>
+          <xsd:enumeration value="Needs Review"/>
+          <xsd:enumeration value="A Violation"/>
+          <xsd:enumeration value="Unpublished Violation"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Best Bets"/>
+          <xsd:enumeration value="Expire"/>
+          <xsd:enumeration value="Hide"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Template"/>
+          <xsd:enumeration value="Training"/>
+          <xsd:enumeration value="URL"/>
+          <xsd:enumeration value="None"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Lookup"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="14"/>
+          <xsd:enumeration value="15"/>
+          <xsd:enumeration value="16"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Hide on web"/>
+          <xsd:enumeration value="On Web no search"/>
+          <xsd:enumeration value="Show everywhere"/>
+          <xsd:enumeration value="Special use only"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Localize"/>
+          <xsd:enumeration value="Never Localize"/>
+          <xsd:enumeration value="Priority Localize"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Downloads xmlns="2958f784-0ef9-4616-b22d-512a8cad1f0d">0</Downloads>
@@ -3715,1094 +4834,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x010100DE95A0C693CEB341887D38A4A2B58B45040072C752107C5A7B47AA91A1EE638E6F1F" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c98c83416931a21d43ed007fda5e4dd">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2958f784-0ef9-4616-b22d-512a8cad1f0d" xmlns:ns3="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="938018c4f46d99993d20879d4e9ddff8" ns2:_="" ns3:_="">
-    <xsd:import namespace="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <xsd:import namespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:AcquiredFrom" minOccurs="0"/>
-                <xsd:element ref="ns2:UACurrentWords" minOccurs="0"/>
-                <xsd:element ref="ns2:TPApplication" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalLog" minOccurs="0"/>
-                <xsd:element ref="ns2:ApprovalStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetStart" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetExpire" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:IsSearchable" minOccurs="0"/>
-                <xsd:element ref="ns2:AssetType" minOccurs="0"/>
-                <xsd:element ref="ns2:APAuthor" minOccurs="0"/>
-                <xsd:element ref="ns2:AverageRating" minOccurs="0"/>
-                <xsd:element ref="ns2:BlockPublish" minOccurs="0"/>
-                <xsd:element ref="ns2:BugNumber" minOccurs="0"/>
-                <xsd:element ref="ns2:CampaignTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPClientViewer" minOccurs="0"/>
-                <xsd:element ref="ns2:ClipArtFilename" minOccurs="0"/>
-                <xsd:element ref="ns2:TPCommandLine" minOccurs="0"/>
-                <xsd:element ref="ns2:TPComponent" minOccurs="0"/>
-                <xsd:element ref="ns2:ContentItem" minOccurs="0"/>
-                <xsd:element ref="ns2:CrawlForDependencies" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXHash" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXUpdate" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewDate" minOccurs="0"/>
-                <xsd:element ref="ns2:IsDeleted" minOccurs="0"/>
-                <xsd:element ref="ns2:APDescription" minOccurs="0"/>
-                <xsd:element ref="ns2:DirectSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:Downloads" minOccurs="0"/>
-                <xsd:element ref="ns2:DSATActionTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:APEditor" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:EditorialTags" minOccurs="0"/>
-                <xsd:element ref="ns2:TPExecutable" minOccurs="0"/>
-                <xsd:element ref="ns2:FeatureTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:TPFriendlyName" minOccurs="0"/>
-                <xsd:element ref="ns2:FriendlyTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:PrimaryImageGen" minOccurs="0"/>
-                <xsd:element ref="ns2:HandoffToMSDN" minOccurs="0"/>
-                <xsd:element ref="ns2:InProjectListLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPInstallLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:InternalTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReview" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLangReviewer" minOccurs="0"/>
-                <xsd:element ref="ns2:MarketSpecific" minOccurs="0"/>
-                <xsd:element ref="ns2:LastCompleteVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastHandOff" minOccurs="0"/>
-                <xsd:element ref="ns2:LastModifiedDateTime" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPreviewVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishErrorLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishResultLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishAttemptDateLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishedByLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishTimeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LastPublishVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLinkType" minOccurs="0"/>
-                <xsd:element ref="ns2:LegacyData" minOccurs="0"/>
-                <xsd:element ref="ns2:TPLaunchHelpLink" minOccurs="0"/>
-                <xsd:element ref="ns2:LocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocLastLocAttemptVersionTypeLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocManualTestRequired" minOccurs="0"/>
-                <xsd:element ref="ns2:LocMarketGroupTiers2" minOccurs="0"/>
-                <xsd:element ref="ns2:LocNewPublishedVersionLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallHandbackStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallLocStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPreviewStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocOverallPublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:IntlLocPriority" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForHandoffsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocProcessedForMarketsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedDependentAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocPublishedLinkedAssetsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:LocRecommendedHandoff" minOccurs="0"/>
-                <xsd:element ref="ns2:LocalizationTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:MachineTranslated" minOccurs="0"/>
-                <xsd:element ref="ns2:Manager" minOccurs="0"/>
-                <xsd:element ref="ns2:Markets" minOccurs="0"/>
-                <xsd:element ref="ns2:Milestone" minOccurs="0"/>
-                <xsd:element ref="ns2:TPNamespace" minOccurs="0"/>
-                <xsd:element ref="ns2:NumericId" minOccurs="0"/>
-                <xsd:element ref="ns2:NumOfRatingsLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:OOCacheId" minOccurs="0"/>
-                <xsd:element ref="ns2:OpenTemplate" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginAsset" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalRelease" minOccurs="0"/>
-                <xsd:element ref="ns2:OriginalSourceMarket" minOccurs="0"/>
-                <xsd:element ref="ns2:OutputCachingOn" minOccurs="0"/>
-                <xsd:element ref="ns2:ParentAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:PlannedPubDate" minOccurs="0"/>
-                <xsd:element ref="ns2:PolicheckWords" minOccurs="0"/>
-                <xsd:element ref="ns2:BusinessGroup" minOccurs="0"/>
-                <xsd:element ref="ns2:UAProjectedTotalWords" minOccurs="0"/>
-                <xsd:element ref="ns2:Provider" minOccurs="0"/>
-                <xsd:element ref="ns2:Providers" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishStatusLookup" minOccurs="0"/>
-                <xsd:element ref="ns2:PublishTargets" minOccurs="0"/>
-                <xsd:element ref="ns2:RecommendationsModifier" minOccurs="0"/>
-                <xsd:element ref="ns2:ArtSampleDocs" minOccurs="0"/>
-                <xsd:element ref="ns2:ScenarioTagsTaxHTField0" minOccurs="0"/>
-                <xsd:element ref="ns2:ShowIn" minOccurs="0"/>
-                <xsd:element ref="ns2:SourceTitle" minOccurs="0"/>
-                <xsd:element ref="ns2:CSXSubmissionDate" minOccurs="0"/>
-                <xsd:element ref="ns2:SubmitterId" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateStatus" minOccurs="0"/>
-                <xsd:element ref="ns2:TemplateTemplateType" minOccurs="0"/>
-                <xsd:element ref="ns2:ThumbnailAssetId" minOccurs="0"/>
-                <xsd:element ref="ns2:TimesCloned" minOccurs="0"/>
-                <xsd:element ref="ns2:TrustLevel" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocComments" minOccurs="0"/>
-                <xsd:element ref="ns2:UALocRecommendation" minOccurs="0"/>
-                <xsd:element ref="ns2:UANotes" minOccurs="0"/>
-                <xsd:element ref="ns2:TPAppVersion" minOccurs="0"/>
-                <xsd:element ref="ns2:VoteCount" minOccurs="0"/>
-                <xsd:element ref="ns3:Description0" minOccurs="0"/>
-                <xsd:element ref="ns3:Component" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2958f784-0ef9-4616-b22d-512a8cad1f0d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="AcquiredFrom" ma:index="1" nillable="true" ma:displayName="Acquired From" ma:default="Internal MS" ma:internalName="AcquiredFrom" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Internal MS"/>
-          <xsd:enumeration value="Community"/>
-          <xsd:enumeration value="MVP"/>
-          <xsd:enumeration value="Publisher"/>
-          <xsd:enumeration value="Partner"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UACurrentWords" ma:index="2" nillable="true" ma:displayName="Actual Word Count" ma:default="" ma:internalName="UACurrentWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPApplication" ma:index="3" nillable="true" ma:displayName="Application to Open Template With" ma:default="" ma:internalName="TPApplication">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalLog" ma:index="4" nillable="true" ma:displayName="Approval Log" ma:default="" ma:hidden="true" ma:internalName="ApprovalLog" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ApprovalStatus" ma:index="5" nillable="true" ma:displayName="Approval Status" ma:default="InProgress" ma:internalName="ApprovalStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="InProgress"/>
-          <xsd:enumeration value="Rejected"/>
-          <xsd:enumeration value="Questionable"/>
-          <xsd:enumeration value="ApprovedAutomatic"/>
-          <xsd:enumeration value="ApprovedManual"/>
-          <xsd:enumeration value="On Hold"/>
-          <xsd:enumeration value="Needs Review"/>
-          <xsd:enumeration value="A Violation"/>
-          <xsd:enumeration value="Unpublished Violation"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetStart" ma:index="6" nillable="true" ma:displayName="Asset Begin Date" ma:default="[Today]" ma:internalName="AssetStart" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetExpire" ma:index="7" nillable="true" ma:displayName="Asset End Date" ma:default="2029-01-01T00:00:00Z" ma:internalName="AssetExpire" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetId" ma:index="8" nillable="true" ma:displayName="Asset ID" ma:default="" ma:indexed="true" ma:internalName="AssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsSearchable" ma:index="9" nillable="true" ma:displayName="Asset Searchable?" ma:default="true" ma:internalName="IsSearchable" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="AssetType" ma:index="10" nillable="true" ma:displayName="Asset Type" ma:default="" ma:internalName="AssetType" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APAuthor" ma:index="11" nillable="true" ma:displayName="Author" ma:default="" ma:list="UserInfo" ma:internalName="APAuthor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="AverageRating" ma:index="12" nillable="true" ma:displayName="Average Rating" ma:internalName="AverageRating" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BlockPublish" ma:index="13" nillable="true" ma:displayName="Block from Publishing?" ma:default="" ma:internalName="BlockPublish" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BugNumber" ma:index="14" nillable="true" ma:displayName="Bug Number" ma:default="" ma:internalName="BugNumber" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CampaignTagsTaxHTField0" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="CampaignTagsTaxHTField0" ma:taxonomyFieldName="CampaignTags" ma:displayName="Campaigns" ma:readOnly="false" ma:default="" ma:fieldId="{ca69c71e-a029-4733-aca1-cabc27411b08}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="ca0e50d4-faa1-44ce-961e-bb1441c60e66" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPClientViewer" ma:index="17" nillable="true" ma:displayName="Client Viewer" ma:default="" ma:internalName="TPClientViewer">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ClipArtFilename" ma:index="18" nillable="true" ma:displayName="Clip Art Name" ma:default="" ma:internalName="ClipArtFilename" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPCommandLine" ma:index="19" nillable="true" ma:displayName="Command Line" ma:default="" ma:internalName="TPCommandLine">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPComponent" ma:index="20" nillable="true" ma:displayName="Component" ma:default="" ma:internalName="TPComponent">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ContentItem" ma:index="21" nillable="true" ma:displayName="Content Item" ma:default="" ma:hidden="true" ma:internalName="ContentItem" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CrawlForDependencies" ma:index="23" nillable="true" ma:displayName="Crawl for Dependencies?" ma:default="true" ma:internalName="CrawlForDependencies" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXHash" ma:index="26" nillable="true" ma:displayName="CSX Hash" ma:default="" ma:indexed="true" ma:internalName="CSXHash" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionMarket" ma:index="27" nillable="true" ma:displayName="CSX Submission Market" ma:default="" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="CSXSubmissionMarket" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXUpdate" ma:index="28" nillable="true" ma:displayName="CSX Updated?" ma:default="false" ma:internalName="CSXUpdate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewDate" ma:index="29" nillable="true" ma:displayName="Date to Complete Intl QA" ma:default="" ma:internalName="IntlLangReviewDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IsDeleted" ma:index="30" nillable="true" ma:displayName="Deleted?" ma:default="" ma:internalName="IsDeleted" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APDescription" ma:index="31" nillable="true" ma:displayName="Description" ma:default="" ma:internalName="APDescription" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DirectSourceMarket" ma:index="32" nillable="true" ma:displayName="Direct Source Market Group" ma:default="" ma:internalName="DirectSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Downloads" ma:index="33" nillable="true" ma:displayName="Downloads" ma:default="0" ma:hidden="true" ma:internalName="Downloads" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="DSATActionTaken" ma:index="34" nillable="true" ma:displayName="DSAT Action Taken" ma:default="" ma:internalName="DSATActionTaken" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Best Bets"/>
-          <xsd:enumeration value="Expire"/>
-          <xsd:enumeration value="Hide"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="APEditor" ma:index="35" nillable="true" ma:displayName="Editor" ma:default="" ma:list="UserInfo" ma:internalName="APEditor" ma:readOnly="false">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:User">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="EditorialStatus" ma:index="36" nillable="true" ma:displayName="Editorial Status" ma:default="" ma:internalName="EditorialStatus" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="EditorialTags" ma:index="37" nillable="true" ma:displayName="Editorial Tags" ma:default="" ma:internalName="EditorialTags">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPExecutable" ma:index="38" nillable="true" ma:displayName="Executable" ma:default="" ma:internalName="TPExecutable">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FeatureTagsTaxHTField0" ma:index="40" nillable="true" ma:taxonomy="true" ma:internalName="FeatureTagsTaxHTField0" ma:taxonomyFieldName="FeatureTags" ma:displayName="Features" ma:readOnly="false" ma:default="" ma:fieldId="{9327d1a0-1a14-4b12-a74c-0f320f972977}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="f1ab6845-967d-4854-a0ba-4ec07f0f8113" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPFriendlyName" ma:index="41" nillable="true" ma:displayName="Friendly Name" ma:default="" ma:internalName="TPFriendlyName">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="FriendlyTitle" ma:index="42" nillable="true" ma:displayName="Friendly Title" ma:default="" ma:description="Shorter title to be used when displaying search results" ma:internalName="FriendlyTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PrimaryImageGen" ma:index="43" nillable="true" ma:displayName="Generate Images?" ma:default="true" ma:internalName="PrimaryImageGen">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="HandoffToMSDN" ma:index="44" nillable="true" ma:displayName="Handoff To MSDN Date" ma:default="" ma:internalName="HandoffToMSDN" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InProjectListLookup" ma:index="45" nillable="true" ma:displayName="InProjectListLookup" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="InProjectListLookup" ma:readOnly="true" ma:showField="InProjectList" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPInstallLocation" ma:index="46" nillable="true" ma:displayName="Install Location" ma:default="" ma:internalName="TPInstallLocation">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="InternalTagsTaxHTField0" ma:index="48" nillable="true" ma:taxonomy="true" ma:internalName="InternalTagsTaxHTField0" ma:taxonomyFieldName="InternalTags" ma:displayName="Internal Tags" ma:readOnly="false" ma:default="" ma:fieldId="{3b364bcb-a06e-4da1-8475-f5243c3236b2}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="82b6639e-f7fc-4c18-ad2d-003a6e707765" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="IntlLangReview" ma:index="49" nillable="true" ma:displayName="Intl Lang QA Review Required?" ma:default="" ma:internalName="IntlLangReview" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLangReviewer" ma:index="50" nillable="true" ma:displayName="Intl Lang QA Reviewer" ma:default="" ma:internalName="IntlLangReviewer" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MarketSpecific" ma:index="51" nillable="true" ma:displayName="Is Market Specific?" ma:default="" ma:internalName="MarketSpecific" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastCompleteVersionLookup" ma:index="52" nillable="true" ma:displayName="Last Complete Version Lookup" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastCompleteVersionLookup" ma:readOnly="true" ma:showField="LastCompleteVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastHandOff" ma:index="53" nillable="true" ma:displayName="Last Hand-off" ma:default="" ma:internalName="LastHandOff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastModifiedDateTime" ma:index="54" nillable="true" ma:displayName="Last Modified Date" ma:default="" ma:internalName="LastModifiedDateTime" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastPreviewErrorLookup" ma:index="55" nillable="true" ma:displayName="Last Preview Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewErrorLookup" ma:readOnly="true" ma:showField="LastPreviewError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewResultLookup" ma:index="56" nillable="true" ma:displayName="Last Preview Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewResultLookup" ma:readOnly="true" ma:showField="LastPreviewResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewAttemptDateLookup" ma:index="57" nillable="true" ma:displayName="Last Preview Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewAttemptDateLookup" ma:readOnly="true" ma:showField="LastPreviewAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewedByLookup" ma:index="58" nillable="true" ma:displayName="Last Previewed By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewedByLookup" ma:readOnly="true" ma:showField="LastPreviewedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewTimeLookup" ma:index="59" nillable="true" ma:displayName="Last Previewed Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewTimeLookup" ma:readOnly="true" ma:showField="LastPreviewTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPreviewVersionLookup" ma:index="60" nillable="true" ma:displayName="Last Previewed Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPreviewVersionLookup" ma:readOnly="true" ma:showField="LastPreviewVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishErrorLookup" ma:index="61" nillable="true" ma:displayName="Last Publish Attempt Error" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishErrorLookup" ma:readOnly="true" ma:showField="LastPublishError" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishResultLookup" ma:index="62" nillable="true" ma:displayName="Last Publish Attempt Result" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishResultLookup" ma:readOnly="true" ma:showField="LastPublishResult" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishAttemptDateLookup" ma:index="63" nillable="true" ma:displayName="Last Publish Attempted On" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishAttemptDateLookup" ma:readOnly="true" ma:showField="LastPublishAttemptDate" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishedByLookup" ma:index="64" nillable="true" ma:displayName="Last Published By" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishedByLookup" ma:readOnly="true" ma:showField="LastPublishedBy" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishTimeLookup" ma:index="65" nillable="true" ma:displayName="Last Published Date" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishTimeLookup" ma:readOnly="true" ma:showField="LastPublishTime" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="LastPublishVersionLookup" ma:index="66" nillable="true" ma:displayName="Last Published Version" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="LastPublishVersionLookup" ma:readOnly="true" ma:showField="LastPublishVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLinkType" ma:index="67" nillable="true" ma:displayName="Launch Help Link Type" ma:default="Template" ma:internalName="TPLaunchHelpLinkType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Template"/>
-          <xsd:enumeration value="Training"/>
-          <xsd:enumeration value="URL"/>
-          <xsd:enumeration value="None"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LegacyData" ma:index="68" nillable="true" ma:displayName="Legacy Data" ma:default="" ma:internalName="LegacyData" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPLaunchHelpLink" ma:index="69" nillable="true" ma:displayName="Link to Launch Help Topic" ma:default="" ma:internalName="TPLaunchHelpLink">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocComments" ma:index="70" nillable="true" ma:displayName="Loc Approval Comments" ma:default="" ma:internalName="LocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionLookup" ma:index="71" nillable="true" ma:displayName="Loc Last Loc Attempt Version" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionLookup" ma:readOnly="false" ma:showField="LastLocAttemptVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocLastLocAttemptVersionTypeLookup" ma:index="72" nillable="true" ma:displayName="Loc Last Loc Attempt Version Type" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocLastLocAttemptVersionTypeLookup" ma:readOnly="true" ma:showField="LastLocAttemptVersionType" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocManualTestRequired" ma:index="73" nillable="true" ma:displayName="Loc Manual Test Required" ma:default="" ma:internalName="LocManualTestRequired" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocMarketGroupTiers2" ma:index="74" nillable="true" ma:displayName="Loc Market Group Tiers" ma:internalName="LocMarketGroupTiers2" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocNewPublishedVersionLookup" ma:index="75" nillable="true" ma:displayName="Loc New Published Version Lookup" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocNewPublishedVersionLookup" ma:readOnly="true" ma:showField="NewPublishedVersion" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallHandbackStatusLookup" ma:index="76" nillable="true" ma:displayName="Loc Overall Handback Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallHandbackStatusLookup" ma:readOnly="true" ma:showField="OverallHandbackStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallLocStatusLookup" ma:index="77" nillable="true" ma:displayName="Loc Overall Localize Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallLocStatusLookup" ma:readOnly="true" ma:showField="OverallLocStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPreviewStatusLookup" ma:index="78" nillable="true" ma:displayName="Loc Overall Preview Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPreviewStatusLookup" ma:readOnly="true" ma:showField="OverallPreviewStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocOverallPublishStatusLookup" ma:index="79" nillable="true" ma:displayName="Loc Overall Publish Status" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocOverallPublishStatusLookup" ma:readOnly="true" ma:showField="OverallPublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="IntlLocPriority" ma:index="80" nillable="true" ma:displayName="Loc Priority" ma:default="" ma:internalName="IntlLocPriority" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForHandoffsLookup" ma:index="81" nillable="true" ma:displayName="Loc Processed For Handoffs" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForHandoffsLookup" ma:readOnly="true" ma:showField="ProcessedForHandoffs" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocProcessedForMarketsLookup" ma:index="82" nillable="true" ma:displayName="Loc Processed For Markets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocProcessedForMarketsLookup" ma:readOnly="true" ma:showField="ProcessedForMarkets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedDependentAssetsLookup" ma:index="83" nillable="true" ma:displayName="Loc Published Dependent Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedDependentAssetsLookup" ma:readOnly="true" ma:showField="PublishedDependentAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocPublishedLinkedAssetsLookup" ma:index="84" nillable="true" ma:displayName="Loc Published Linked Assets" ma:default="" ma:list="{AC64899A-88C0-4725-BCFC-902FA402DE74}" ma:internalName="LocPublishedLinkedAssetsLookup" ma:readOnly="true" ma:showField="PublishedLinkedAssets" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Lookup"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocRecommendedHandoff" ma:index="85" nillable="true" ma:displayName="Loc Recommended Handoff" ma:default="" ma:indexed="true" ma:internalName="LocRecommendedHandoff" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LocalizationTagsTaxHTField0" ma:index="87" nillable="true" ma:taxonomy="true" ma:internalName="LocalizationTagsTaxHTField0" ma:taxonomyFieldName="LocalizationTags" ma:displayName="Localization Tags" ma:readOnly="false" ma:default="" ma:fieldId="{251ee2d3-c117-4524-b3f1-1010c3cab2a3}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="5b7703a5-8e8b-4b58-8b31-1cea35331da3" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MachineTranslated" ma:index="88" nillable="true" ma:displayName="Machine Translated" ma:default="" ma:internalName="MachineTranslated" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Manager" ma:index="89" nillable="true" ma:displayName="Manager" ma:hidden="true" ma:internalName="Manager" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Markets" ma:index="90" nillable="true" ma:displayName="Markets" ma:default="" ma:description="Leave blank to show in all markets" ma:list="{8D80075B-F8CE-48D6-9BD2-D195F7E115A9}" ma:internalName="Markets" ma:readOnly="false" ma:showField="MarketName" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="Milestone" ma:index="91" nillable="true" ma:displayName="Milestone" ma:default="" ma:internalName="Milestone" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPNamespace" ma:index="94" nillable="true" ma:displayName="Namespace" ma:default="" ma:internalName="TPNamespace">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumericId" ma:index="95" nillable="true" ma:displayName="Numeric ID" ma:default="" ma:indexed="true" ma:internalName="NumericId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="NumOfRatingsLookup" ma:index="96" nillable="true" ma:displayName="NumOfRatings" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="NumOfRatingsLookup" ma:readOnly="true" ma:showField="NumOfRatings" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="OOCacheId" ma:index="97" nillable="true" ma:displayName="OOCacheId" ma:internalName="OOCacheId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OpenTemplate" ma:index="98" nillable="true" ma:displayName="Open Template" ma:default="true" ma:internalName="OpenTemplate">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginAsset" ma:index="99" nillable="true" ma:displayName="Origin Asset" ma:default="" ma:internalName="OriginAsset" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalRelease" ma:index="100" nillable="true" ma:displayName="Original Release" ma:default="15" ma:internalName="OriginalRelease" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="14"/>
-          <xsd:enumeration value="15"/>
-          <xsd:enumeration value="16"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OriginalSourceMarket" ma:index="101" nillable="true" ma:displayName="Original Source Market Group" ma:default="" ma:internalName="OriginalSourceMarket" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="OutputCachingOn" ma:index="102" nillable="true" ma:displayName="Output Caching" ma:default="true" ma:hidden="true" ma:internalName="OutputCachingOn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Boolean"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ParentAssetId" ma:index="103" nillable="true" ma:displayName="Parent Asset Id" ma:default="" ma:internalName="ParentAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PlannedPubDate" ma:index="104" nillable="true" ma:displayName="Planned Publish Date" ma:default="" ma:indexed="true" ma:internalName="PlannedPubDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PolicheckWords" ma:index="105" nillable="true" ma:displayName="Policheck Words" ma:default="" ma:internalName="PolicheckWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="BusinessGroup" ma:index="106" nillable="true" ma:displayName="Product Division Owner" ma:default="" ma:internalName="BusinessGroup" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UAProjectedTotalWords" ma:index="107" nillable="true" ma:displayName="Projected Word Count" ma:default="" ma:internalName="UAProjectedTotalWords" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Provider" ma:index="108" nillable="true" ma:displayName="Provider" ma:default="" ma:internalName="Provider" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Providers" ma:index="109" nillable="true" ma:displayName="Providers" ma:default="" ma:internalName="Providers">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="PublishStatusLookup" ma:index="110" nillable="true" ma:displayName="Publish Status" ma:default="" ma:list="{1F044C38-11A0-4051-9DF8-A3AFA85E16DC}" ma:internalName="PublishStatusLookup" ma:readOnly="false" ma:showField="PublishStatus" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="PublishTargets" ma:index="111" nillable="true" ma:displayName="Publish Target" ma:default="OfficeOnlineVNext" ma:internalName="PublishTargets" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="RecommendationsModifier" ma:index="112" nillable="true" ma:displayName="Recommendations Modifier" ma:default="" ma:internalName="RecommendationsModifier" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ArtSampleDocs" ma:index="113" nillable="true" ma:displayName="Sample Docs" ma:default="" ma:hidden="true" ma:internalName="ArtSampleDocs" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ScenarioTagsTaxHTField0" ma:index="115" nillable="true" ma:taxonomy="true" ma:internalName="ScenarioTagsTaxHTField0" ma:taxonomyFieldName="ScenarioTags" ma:displayName="Scenarios" ma:readOnly="false" ma:default="" ma:fieldId="{654e2ea7-8c43-4b3c-9db4-bd71f7cfe4f4}" ma:taxonomyMulti="true" ma:sspId="8f79753a-75d3-41f5-8ca3-40b843941b4f" ma:termSetId="4b7d5f16-e2f2-4fc0-bab3-6e8b931e57d6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="ShowIn" ma:index="117" nillable="true" ma:displayName="Show In" ma:default="Show everywhere" ma:internalName="ShowIn" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Hide on web"/>
-          <xsd:enumeration value="On Web no search"/>
-          <xsd:enumeration value="Show everywhere"/>
-          <xsd:enumeration value="Special use only"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SourceTitle" ma:index="118" nillable="true" ma:displayName="Source Title" ma:default="" ma:indexed="true" ma:internalName="SourceTitle" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="CSXSubmissionDate" ma:index="119" nillable="true" ma:displayName="Submission Date" ma:default="" ma:internalName="CSXSubmissionDate" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SubmitterId" ma:index="120" nillable="true" ma:displayName="Submitter ID" ma:default="" ma:internalName="SubmitterId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="121" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAllLabel" ma:index="122" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{33f01220-6030-4880-975f-b9ea0de09f53}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2958f784-0ef9-4616-b22d-512a8cad1f0d">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="TemplateStatus" ma:index="123" nillable="true" ma:displayName="Template Status" ma:default="" ma:internalName="TemplateStatus">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TemplateTemplateType" ma:index="124" nillable="true" ma:displayName="Template Type" ma:default="" ma:internalName="TemplateTemplateType">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="ThumbnailAssetId" ma:index="125" nillable="true" ma:displayName="Thumbnail Image Asset" ma:default="" ma:internalName="ThumbnailAssetId" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TimesCloned" ma:index="126" nillable="true" ma:displayName="Times Cloned" ma:default="" ma:internalName="TimesCloned" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Number"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TrustLevel" ma:index="128" nillable="true" ma:displayName="Trust Level" ma:default="1 Microsoft Managed Content" ma:internalName="TrustLevel" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocComments" ma:index="129" nillable="true" ma:displayName="UA Loc Comments" ma:default="" ma:internalName="UALocComments" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UALocRecommendation" ma:index="130" nillable="true" ma:displayName="UA Loc Recommendation" ma:default="Localize" ma:internalName="UALocRecommendation" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Choice">
-          <xsd:enumeration value="Localize"/>
-          <xsd:enumeration value="Never Localize"/>
-          <xsd:enumeration value="Priority Localize"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="UANotes" ma:index="131" nillable="true" ma:displayName="UA Notes" ma:default="" ma:internalName="UANotes" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TPAppVersion" ma:index="132" nillable="true" ma:displayName="Version" ma:default="" ma:internalName="TPAppVersion">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="VoteCount" ma:index="133" nillable="true" ma:displayName="Vote Count" ma:default="" ma:internalName="VoteCount" ma:readOnly="false">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb5acd76-e9f3-4601-9d69-91f53ab96ae6" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="Description0" ma:index="134" nillable="true" ma:displayName="Description" ma:internalName="Description0">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Component" ma:index="135" nillable="true" ma:displayName="Component" ma:internalName="Component">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="22" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="127" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
-    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3E314C6-CC6F-4B8C-BA77-46BFB16C292A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4819,4 +4851,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDB0ABD9-2D20-4762-A9C4-40EB18F83CA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8121883-470C-4C1A-AD2C-C9FFF4CD7655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2958f784-0ef9-4616-b22d-512a8cad1f0d"/>
+    <ds:schemaRef ds:uri="fb5acd76-e9f3-4601-9d69-91f53ab96ae6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>